<commit_message>
added weeks date computation
</commit_message>
<xml_diff>
--- a/scrapers_pack/fetcher_temp/temp.xlsx
+++ b/scrapers_pack/fetcher_temp/temp.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +57,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,1413 +455,1487 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A2" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nearly 200 EU observers to monitor May 12 polls</t>
+          <t>MGen’s Manny Rubio urges power investments after Spain, Portugal blackouts</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/nearly-200-eu-observers-to-monitor-may-12-polls/</t>
+          <t>https://bilyonaryo.com/2025/05/01/mgens-manny-rubio-urges-power-investments-after-spain-portugal-blackouts/power/</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A3" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Marcos declares period of national mourning for Pope</t>
+          <t>South’s rising stars aim to take spotlight in JPGT Mactan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/marcos-declares-period-of-national-mourning-for-pope/</t>
+          <t>https://bilyonaryo.com/2025/05/01/souths-rising-stars-aim-to-take-spotlight-in-jpgt-mactan/golf/</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A4" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Presidential Medal of Merit for Aunor, Corrales, 2 others</t>
+          <t>Willy Ocier-led LOTO rethinks online gaming investment amid uncertain future</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/presidential-medal-of-merit-for-aunor-corrales-2-others/</t>
+          <t>https://bilyonaryo.com/2025/05/01/willy-ocier-led-loto-rethinks-online-gaming-investment-amid-uncertain-future/gaming/</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A5" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Impeachment not a confidence game, Sara told</t>
+          <t>Dizon grounds Chua-owned Solid North Bus line after deadly expressway crash</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/impeachment-not-a-confidence-game-sara-told/</t>
+          <t>https://bilyonaryo.com/2025/05/01/dizon-grounds-chua-owned-solid-north-bus-line-after-deadly-expressway-crash/business/</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A6" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Defense counsel slams govt for surrendering Duterte to ICC</t>
+          <t>Political hit job? Vincent Reyes’ mother slams ‘baseless’ allegations ahead of elections</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/defense-counsel-slams-govt-for-surrendering-duterte-to-icc/</t>
+          <t>https://bilyonaryo.com/2025/05/01/political-hit-job-vincent-reyes-mother-slams-baseless-allegations-ahead-of-elections/business/</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A7" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Japanese premier visits Manila on April 29</t>
+          <t>Riding the cloud wave: Philippines sets 1GW data center goal for 2029</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/japanese-premier-visits-manila-on-april-29/</t>
+          <t>https://bilyonaryo.com/2025/05/01/riding-the-cloud-wave-philippines-sets-1gw-data-center-goal-for-2029/technology/</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A8" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ex-CA justice charged for gross misconduct over 2020 killing IN Cebu</t>
+          <t>Rebuilding EDSA Busway: DOTr sets P253M bid for station upgrades</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/ex-ca-justice-charged-for-gross-misconduct-over-2020-killing-in-cebu/</t>
+          <t>https://bilyonaryo.com/2025/05/01/rebuilding-edsa-busway-dotr-sets-p253m-bid-for-station-upgrades/headlines/</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A9" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Comelec cancels PBBM party-list registration</t>
+          <t>Manila Bay reclamation on track for 2028, Sy-blings set to begin next phase of development</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/comelec-cancels-pbbm-party-list-registration/</t>
+          <t>https://bilyonaryo.com/2025/05/01/manila-bay-reclamation-on-track-for-2028-sy-blings-set-to-begin-next-phase-of-development/property/</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A10" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PBBM urged to realign budget to Mindanao to spur growth</t>
+          <t>Digital peacekeepers: Aguda-led DICT and Google strengthen alliance to wipe out fake news in PH cyberspace</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/pbbm-urged-to-realign-budget-to-mindanao-to-spur-growth/</t>
+          <t>https://bilyonaryo.com/2025/05/01/digital-peacekeepers-aguda-led-dict-and-google-strengthen-alliance-to-wipe-out-fake-news-in-ph-cyberspace/technology/</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A11" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Former Marine officer to collect P4M cash benefits 17 years after retirement</t>
+          <t>Star Horse shipping owners on the run? Quezon mayor bet Vincent Reyes, 3 relatives wanted for P33M estafa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/former-marine-officer-to-collect-p4m-cash-benefits-17-years-after-retirement/</t>
+          <t>https://bilyonaryo.com/2025/05/01/star-horse-shipping-owners-on-the-run-quezon-mayor-bet-vincent-reyes-3-relatives-wanted-for-p33m-estafa/business/</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A12" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Govt employees told to file SALNs</t>
+          <t>Di nyo naman ikahihirap yan! Tiny chili oil portion triggers Chowking roast fest</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/govt-employees-told-to-file-salns/</t>
+          <t>https://bilyonaryo.com/2025/05/01/di-nyo-naman-ikahihirap-yan-tiny-chili-oil-portion-triggers-chowking-roast-fest/food/</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A13" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Crackdown on reckless PUV operators, drivers intensified</t>
+          <t>Congrats Tatay Digz! Shakey’s gets trolled for promo winner sharing initials with ex-President</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/crackdown-on-reckless-puv-operators-drivers-intensified/</t>
+          <t>https://bilyonaryo.com/2025/05/01/congrats-tatay-digz-shakeys-gets-trolled-for-promo-winner-sharing-initials-with-ex-president/food/</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A14" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SC cautions public vs fake court orders</t>
+          <t>Cathay Pacific under fire: Dizon probes damaged passport incident in Cebu</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/sc-cautions-public-vs-fake-court-orders/</t>
+          <t>https://bilyonaryo.com/2025/05/01/cathay-pacific-under-fire-dizon-probes-damaged-passport-incident-in-cebu/travel/</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A15" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SE Asia faces ‘significant shock’ from US tariffs; PH growth forecast cut — ANZ</t>
+          <t>SEC’s Francisco calls on companies to make ESG a habit, not a hurdle</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/business-news/se-asia-faces-significant-shock-from-us-tariffs-ph-growth-forecast-cut-anz/</t>
+          <t>https://bilyonaryo.com/2025/05/01/secs-francisco-calls-on-companies-to-make-esg-a-habit-not-a-hurdle/business/</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A16" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>‘Luffy gang’ member nabbed in Las Piñas</t>
+          <t>Curtain call: Lopez family’s film restoration unit bows out after 14 years</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/luffy-gang-member-nabbed-in-las-pinas/</t>
+          <t>https://bilyonaryo.com/2025/05/01/curtain-call-lopez-familys-film-restoration-unit-bows-out-after-14-years/entertainment/</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A17" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PH risks missing trade advantage without quick policy response — PIDS</t>
+          <t>Ayala Land’s Southern charm: How four estates are transforming Laguna and Cavite</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/business-news/ph-risks-missing-trade-advantage-without-quick-policy-response-pids/</t>
+          <t>https://bilyonaryo.com/2025/05/01/ayala-lands-southern-charm-how-four-estates-are-transforming-laguna-and-cavite/property/</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A18" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cyber libel raps vs Harry Roque junked</t>
+          <t>Aboitiz Group Q1 profit falls 35% in Q1; power still king amid sector-wide pressures</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/cyber-libel-raps-vs-harry-roque-junked/</t>
+          <t>https://bilyonaryo.com/2025/05/01/aboitiz-group-q1-profit-fall-35-in-q1-power-still-king-amid-sector-wide-pressures/business/</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A19" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cyber libel raps vs Harry Roque junked</t>
+          <t>Netflix’s ‘The Eternaut’ echoes fight against tyranny: actor Ricardo Darin</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/cyber-libel-raps-vs-harry-roque-junked/</t>
+          <t>https://bilyonaryo.com/2025/05/01/netflixs-the-eternaut-echoes-fight-against-tyranny-actor-ricardo-darin/entertainment/</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A20" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PH export orders on hold pending US tariffs’ 90-day suspension: Port users warn of risks</t>
+          <t>Meta quarterly profit climbs despite big cloud spending</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/business-news/ph-export-orders-on-hold-pending-us-tariffs-90-day-suspension-port-users-warn-of-risks/</t>
+          <t>https://bilyonaryo.com/2025/05/01/meta-quarterly-profit-climbs-despite-big-cloud-spending/technology/</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A21" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Napolcom to revisit PNP recruitment system</t>
+          <t>Microsoft reports strong results driven by cloud and AI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/napolcom-to-revisit-pnp-recruitment-system/</t>
+          <t>https://bilyonaryo.com/2025/05/01/microsoft-reports-strong-results-driven-by-cloud-and-ai/technology/</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A22" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PH stocks buoyed by Wall St rally as Trump softens stance on China</t>
+          <t>Catalonia delays raising tourist tax until after summer</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/business-news/ph-stocks-buoyed-by-wall-st-rally-as-trump-softens-stance-on-china/</t>
+          <t>https://bilyonaryo.com/2025/05/01/catalonia-delays-raising-tourist-tax-until-after-summer/travel/</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A23" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SC: Barangays can hold fund raiser bingo games without Pagcor permit</t>
+          <t>Spain’s grid denies dependence on solar power to blame for blackout</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/sc-barangays-can-hold-fund-raiser-bingo-games-without-pagcor-permit/</t>
+          <t>https://bilyonaryo.com/2025/05/01/spains-grid-denies-dependence-on-solar-power-to-blame-for-blackout/power/</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A24" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5 of 26 Pinoys rescued from scam hub in Cambodia tagged as recruiters</t>
+          <t>King Charles says cancer diagnosis has shown him ‘the very best of humanity’</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/5-of-26-pinoys-rescued-from-scam-hub-in-cambodia-tagged-as-recruiters/</t>
+          <t>https://bilyonaryo.com/2025/05/01/king-charles-says-cancer-diagnosis-has-shown-him-the-very-best-of-humanity/royals/</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A25" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lack of infra a challenge for PH tourism— Europe business group</t>
+          <t>Visa partners with AI giants to streamline online shopping</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/business-news/lack-of-infra-a-challenge-for-ph-tourism-europe-business-group/</t>
+          <t>https://bilyonaryo.com/2025/05/01/visa-partners-with-ai-giants-to-streamline-online-shopping/technology/</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A26" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Is Open Finance open for all?</t>
+          <t>Wall Street dips as economy contracts for first time since 2022</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/business-news/is-open-finance-open-for-all/</t>
+          <t>https://bilyonaryo.com/2025/05/01/wall-street-dips-as-economy-contracts-for-first-time-since-2022/money/</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A27" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Qatar OFWs warned over ‘indecent acts’ in public</t>
+          <t>Yogurt maker Danone working to remove artificial dyes from products sold in US</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/qatar-ofws-warned-over-indecent-acts-in-public/</t>
+          <t>https://bilyonaryo.com/2025/05/01/yogurt-maker-danone-working-to-remove-artificial-dyes-from-products-sold-in-us/food/</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A28" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>10 QC cops relieved over irregular anti-gambling operation</t>
+          <t>John Elway’s business partner dies from golf cart fall</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/10-qc-cops-relieved-over-irregular-anti-gambling-operation/</t>
+          <t>https://bilyonaryo.com/2025/05/01/john-elways-business-partner-dies-from-golf-cart-fall/golf/</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A29" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>10 QC cops relieved over irregular anti-gambling operation</t>
+          <t>Major airlines ask US to extend cuts to minimum New York flight requirements</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/10-qc-cops-relieved-over-irregular-anti-gambling-operation/</t>
+          <t>https://bilyonaryo.com/2025/05/01/major-airlines-ask-us-to-extend-cuts-to-minimum-new-york-flight-requirements/travel/</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A30" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Marcos inaugurates first AI-ready data center in PH</t>
+          <t>South Korea’s deadly fires made twice as likely by climate change, researchers say</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/corporate/marcos-inaugurates-first-ai-ready-data-center-in-ph/</t>
+          <t>https://bilyonaryo.com/2025/05/01/south-koreas-deadly-fires-made-twice-as-likely-by-climate-change-researchers-say/nature/</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A31" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DOF streamlines tax incentive claims for schools</t>
+          <t>Emirates executive says no impact seen from US tariffs, but airline remains vigilant</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/corporate/dof-streamlines-tax-incentive-claims-for-schools/</t>
+          <t>https://bilyonaryo.com/2025/05/01/emirates-executive-says-no-impact-seen-from-us-tariffs-but-airline-remains-vigilant/travel/</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A32" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Palay-to-rice conversion rate up at 63% from 55% due to new machinery — DA</t>
+          <t>Airbus urges return to zero-tariff deal as Q1 beats forecasts</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/corporate/palay-to-rice-conversion-rate-up-at-63-from-55-due-to-new-machinery-da/</t>
+          <t>https://bilyonaryo.com/2025/05/01/airbus-urges-return-to-zero-tariff-deal-as-q1-beats-forecasts/travel/</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A33" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>PAL appoints British airline exec as new president</t>
+          <t>Trump struggles to explain weak economic data as he reaches 100-day mark</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/corporate/pal-appoints-british-airline-exec-as-new-president/</t>
+          <t>https://bilyonaryo.com/2025/05/01/trump-struggles-to-explain-weak-economic-data-as-he-reaches-100-day-mark/money/</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A34" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ayala’s ACEN to raise P30B via share sale</t>
+          <t>Ford kills project to develop Tesla-like electronic brain</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/corporate/ayalas-acen-to-raise-p30b-via-share-sale/</t>
+          <t>https://bilyonaryo.com/2025/05/01/ford-kills-project-to-develop-tesla-like-electronic-brain/mobility/</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A35" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Eton reports 71.5% drop in 2024 net income</t>
+          <t>Pope Francis interview with Scorsese featured in new documentary</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/corporate/eton-reports-71-5-drop-in-2024-net-income/</t>
+          <t>https://bilyonaryo.com/2025/05/01/pope-francis-interview-with-scorsese-featured-in-new-documentary/entertainment/</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A36" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PH to receive 2nd batch of BrahMos missile system</t>
+          <t>Trump suggests US may not give more grants to Harvard University</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/ph-to-receive-2nd-batch-of-brahmos-missile-system/</t>
+          <t>https://bilyonaryo.com/2025/05/01/trump-suggests-us-may-not-give-more-grants-to-harvard-university/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A37" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Mindanao-born justices named to CA</t>
+          <t>US judge rules Apple violated order to reform App Store</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/mindanao-born-justices-named-to-ca/</t>
+          <t>https://bilyonaryo.com/2025/05/01/us-judge-rules-apple-violated-order-to-reform-app-store/technology/</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A38" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BOJ to raise rates in Q3, analysts say</t>
+          <t>Dizon touts Manila South Harbor’s P5.7B green, high-tech overhaul as key regional trade driver</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/world-business/boj-to-raise-rates-in-q3-analysts-say/</t>
+          <t>https://bilyonaryo.com/2025/05/02/dizon-touts-manila-south-harbors-p5-7b-green-high-tech-overhaul-as-key-regional-trade-driver/business/</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A39" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cop who fired gun in drinking spree arrested</t>
+          <t>Deadly expressway crash: LTFRB freezes Chua’s Solid North fleet, orders P400K payouts for victims</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/cop-who-fired-gun-in-drinking-spree-arrested/</t>
+          <t>https://bilyonaryo.com/2025/05/02/deadly-expressway-crash-ltfrb-freezes-chuas-solid-north-fleet-orders-p400k-payouts-for-victims/headlines/</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A40" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Pinedas of Pampanga endorse Alyansa senatorial candidates</t>
+          <t>Davao River Bridge to open ahead of schedule, promises economic boost and better mobility</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/pinedas-of-pampanga-endorse-alyansa-senatorial-candidates/</t>
+          <t>https://bilyonaryo.com/2025/05/02/davao-river-bridge-to-open-ahead-of-schedule-promises-economic-boost-and-better-mobility/infrastructure/</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A41" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Remember this summer</t>
+          <t>Lucio Tan’s PAL links up with Alaska Airlines to widen network, reward flyers</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/other-sports/remember-this-summer/</t>
+          <t>https://bilyonaryo.com/2025/05/02/lucio-tans-pal-links-up-with-alaska-airlines-to-widen-network-reward-flyers/travel/</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A42" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rizal execs air support for Bam Aquino’s Senate bid </t>
+          <t>Siargao in uproar: Locals accuse Israeli tourists of harassment and economic sabotage</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/rizal-execs-air-support-for-bam-aquinos-senate-bid/</t>
+          <t>https://bilyonaryo.com/2025/05/02/siargao-in-uproar-locals-accuse-israeli-tourists-of-harassment-and-economic-sabotage/travel/</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A43" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Metro Retail reports farm-to-market drive benefits 500 farmers</t>
+          <t>‘We were never consulted’: Cayetano denies Taguig blocked Makati Subway amid dispute</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/market/metro-retail-reports-farm-to-market-drive-benefits-500-farmers/</t>
+          <t>https://bilyonaryo.com/2025/05/02/we-were-never-consulted-cayetano-denies-taguig-blocked-makati-subway-amid-dispute/business/</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A44" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Rody calls for calm, restraint amid growing election tension</t>
+          <t>Netizens rant: Jollibee, bakit ganon? Service abroad vs service here — ang layo!</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/rody-calls-for-calm-restraint-amid-growing-election-tension/</t>
+          <t>https://bilyonaryo.com/2025/05/02/netizens-rant-jollibee-bakit-ganon-service-abroad-vs-service-here-ang-layo/food/</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A45" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>NLEX hands TNT early stunner</t>
+          <t>Vince Perez adds Batangas to Alternergy’s growing green energy map</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/basketball/nlex-hands-tnt-early-stunner/</t>
+          <t>https://bilyonaryo.com/2025/05/02/vince-perez-adds-batangas-to-alternergys-growing-green-energy-map/power/</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A46" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Comelec to closely monitor ‘sample ballots’ ahead of polls</t>
+          <t>Solid 2024: Megawide doubles profit on Saavedra’s strategic moves, lifts order book to P43.5 billion</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/comelec-to-closely-monitor-sample-ballots-ahead-of-polls/</t>
+          <t>https://bilyonaryo.com/2025/05/02/solid-2024-megawide-doubles-profit-on-saavedras-strategic-moves-lifts-order-book-to-p43-5-billion/infrastructure/</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A47" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Stocks, dollar rebound in Asia</t>
+          <t>Puregold’s 2024 Performance Signals Strong Growth and Global Recognition</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/market/stocks-dollar-rebound-in-asia/</t>
+          <t>https://bilyonaryo.com/2025/05/02/puregolds-2024-performance-signals-strong-growth-and-global-recognition/brand-news/</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A48" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Indonesia, PH agree to enhance cooperation</t>
+          <t>Ramon Ang’s BankCom posts solid Q1 on strong corporate lending, FX gains</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/national-news/indonesia-ph-agree-to-enhance-cooperation/</t>
+          <t>https://bilyonaryo.com/2025/05/02/ramon-angs-bankcom-posts-solid-q1-on-strong-corporate-lending-fx-gains/business/</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A49" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Espedido, Sarines extend win streaks</t>
+          <t>P1 million reward for information</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/golf/espedido-sarines-extend-win-streaks/</t>
+          <t>https://bilyonaryo.com/2025/05/02/p1-million-reward-for-information/money/</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A50" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lakers even series vs Wolves</t>
+          <t>Unlocking new growth potential: Frederick Dy’s Security Bank seals P10.4B investment in Home Credit Philippines</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/basketball/lakers-even-series-vs-wolves/</t>
+          <t>https://bilyonaryo.com/2025/05/02/unlocking-new-growth-potential-frederick-dys-security-bank-seals-p10-4b-investment-in-home-credit-philippines/money/</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A51" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>PTA holds taekwondo summer program</t>
+          <t>Challenging start to 2025: Softer coal prices slash Consunji-led Semirara’s earnings by a third</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/other-sports/pta-holds-taekwondo-summer-program/</t>
+          <t>https://bilyonaryo.com/2025/05/02/challenging-start-to-2025-softer-coal-prices-slash-consunji-led-semiraras-earnings-by-a-third/mining/</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A52" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Creamline, PLDT in no-tomorrow games</t>
+          <t>New research reveals where N. American bird populations are crashing</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/volleyball/creamline-pldt-in-no-tomorrow-games/</t>
+          <t>https://bilyonaryo.com/2025/05/02/new-research-reveals-where-n-american-bird-populations-are-crashing/nature/</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A53" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>How will the young guns fare against veteran riders?</t>
+          <t>McDonald’s profits hit by weakness in US market</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/other-sports/how-will-the-young-guns-fare-against-veteran-riders/</t>
+          <t>https://bilyonaryo.com/2025/05/02/mcdonalds-profits-hit-by-weakness-in-us-market/food/</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A54" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Can Eala beat Swiatek again?</t>
+          <t>Amazon revenue climbs 9%, but outlook sends shares lower</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/tennis/can-eala-beat-swiatek-again/</t>
+          <t>https://bilyonaryo.com/2025/05/02/amazon-revenue-climbs-9-but-outlook-sends-shares-lower/technology/</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A55" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cubs rally past Dodgers 11-10 in 10 innings</t>
+          <t>Backyard barnyard: rising egg prices prompt hen hires in US</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/baseball/cubs-rally-past-dodgers-11-10-in-10-innings/</t>
+          <t>https://bilyonaryo.com/2025/05/02/backyard-barnyard-rising-egg-prices-prompt-hen-hires-in-us/food/</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A56" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Lady Generals bring down Lady Cardinals</t>
+          <t>Cat sole survivor of 115-meter fall in US canyon</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/volleyball/lady-generals-bring-down-lady-cardinals/</t>
+          <t>https://bilyonaryo.com/2025/05/02/cat-sole-survivor-of-115-meter-fall-in-us-canyon/nature/</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A57" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Forget the film: Vatican is preparing for the real ‘Conclave’</t>
+          <t>Asian stocks gain after China teases US tariff talks</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/news/international-news/forget-the-film-vatican-is-preparing-for-the-real-conclave/</t>
+          <t>https://bilyonaryo.com/2025/05/02/asian-stocks-gain-after-china-teases-us-tariff-talks/money/</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A58" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Taguig City 4.25 Anniversary Sale</t>
+          <t>Truck driver’s body recovered from huge Japan sinkhole after three months</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/marketing-board/taguig-city-4-25-anniversary-sale/</t>
+          <t>https://bilyonaryo.com/2025/05/02/truck-drivers-body-recovered-from-huge-japan-sinkhole-after-three-months/nature/</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A59" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Max’s balances heritage and progress</t>
+          <t>Harrods is latest British retailer to be hit by cyber attack</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/lifestyle/food/maxs-balances-heritage-and-progress/</t>
+          <t>https://bilyonaryo.com/2025/05/02/harrods-is-latest-british-retailer-to-be-hit-by-cyber-attack/retail/</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A60" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Construction activity declines 2.5% in Feb</t>
+          <t>Nvidia raised concerns about Huawei’s growing AI capabilities with US lawmakers</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/property/construction-activity-declines-2-5-in-feb/</t>
+          <t>https://bilyonaryo.com/2025/05/02/nvidia-raised-concerns-about-huaweis-growing-ai-capabilities-with-us-lawmakers/technology/</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A61" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Golden Tigresses seal Final Four showdown</t>
+          <t>Judge in Meta case warns AI could ‘obliterate’ market for original works</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/volleyball/golden-tigresses-seal-final-four-showdown/</t>
+          <t>https://bilyonaryo.com/2025/05/02/judge-in-meta-case-warns-ai-could-obliterate-market-for-original-works/fine-works/</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A62" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>PAL presents anniversary dessert selection</t>
+          <t>Apple girds for more trade war pain, trims buyback</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/lifestyle/food/pal-presents-anniversary-dessert-selection/</t>
+          <t>https://bilyonaryo.com/2025/05/02/apple-girds-for-more-trade-war-pain-trims-buyback/technology/</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A63" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Pope Francis and a Third World War</t>
+          <t>China ‘evaluating’ US offer to negotiate tariffs; Beijing’s door is ‘open’</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/column-of-the-day/pope-francis-and-a-third-world-war/</t>
+          <t>https://bilyonaryo.com/2025/05/02/china-evaluating-us-offer-to-negotiate-tariffs-beijings-door-is-open/trade/</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A64" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Golden Tigresses seal Final Four showdown</t>
+          <t>US blacklist on China is riddled with errors, outdated details</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/volleyball/golden-tigresses-seal-final-four-showdown/</t>
+          <t>https://bilyonaryo.com/2025/05/02/us-blacklist-on-china-is-riddled-with-errors-outdated-details/trade/</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A65" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Construction activity declines 2.5% in Feb</t>
+          <t>Japan says massive Treasury stockpile among tools for US trade talks</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/property/construction-activity-declines-2-5-in-feb/</t>
+          <t>https://bilyonaryo.com/2025/05/02/japan-says-massive-treasury-stockpile-among-tools-for-us-trade-talks/money/</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A66" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>FC Home Center awards life-changing prize in “Pangarap na Bahay at Lupa Part 2” promo</t>
+          <t>Uyan’s growth playbook delivers for Sy-led Chinabank: Q1 profit jumps 10% on lending and digital push</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/marketing-board/fc-home-center-awards-life-changing-prize-in-pangarap-na-bahay-at-lupa-part-2-promo/</t>
+          <t>https://bilyonaryo.com/2025/05/02/uyans-growth-playbook-delivers-for-sy-led-chinabank-q1-profit-jumps-10-on-lending-and-digital-push/business/</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A67" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>China asks Korea not to supply US with products using rare earths</t>
+          <t>Swipe like a bilyonaryo! MVP’s Maya rops luxe Black Card with PAL Miles &amp; VIP lounge access</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/shipping-transportation/china-asks-korea-not-to-supply-us-with-products-using-rare-earths/</t>
+          <t>https://bilyonaryo.com/2025/05/02/swipe-like-a-bilyonaryo-mvps-maya-rops-luxe-black-card-with-pal-miles-vip-lounge-access/travel/</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A68" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8990 posts lower profit in 2024</t>
+          <t>LTFRB slashes MoveIt Riders by 14,000 — thousands could be out of work</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/property/8990-posts-lower-profit-in-2024/</t>
+          <t>https://bilyonaryo.com/2025/05/02/ltfrb-slashes-moveit-riders-by-14000-thousands-could-be-out-of-work/mobility/</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A69" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Never enough tributes for Nora and Pilita</t>
+          <t>Foodies, brace yourselves! Gordon Ramsay’s Bringing His Heat to Cebu with 2 New Restos in Kevin Tan’s malls</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/entertainment/columns-entertainment/never-enough-tributes-for-nora-and-pilita/</t>
+          <t>https://bilyonaryo.com/2025/05/02/foodies-brace-yourselves-gordon-ramsays-bringing-his-heat-to-cebu-with-2-new-restos-in-kevin-tans-malls/food/</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A70" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Grab strengthens role as gig work leader in the Philippines, honors partners at Saludo Concert</t>
+          <t>Deck Go, Cristina Roque go to Washington to woo US businessmen amid Trump tariff negotiations</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/marketing-board/grab-strengthens-role-as-gig-work-leader-in-the-philippines-honors-partners-at-saludo-concert/</t>
+          <t>https://bilyonaryo.com/2025/05/02/deck-go-cristina-roque-go-to-washington-to-woo-us-businessmen-amid-trump-tariff-negotiations/business/</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A71" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>China asks Korea not to supply US with products using rare earths</t>
+          <t>Scottie Scheffler shoots scorching 61 to lead Byron Nelson</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/shipping-transportation/china-asks-korea-not-to-supply-us-with-products-using-rare-earths/</t>
+          <t>https://bilyonaryo.com/2025/05/02/scottie-scheffler-shoots-scorching-61-to-lead-byron-nelson/golf/</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A72" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Thunder down Grizzlies anew; Pacers beat Bucks</t>
+          <t>Slow and easily beaten — Messi’s Miami project risks global embarrassment</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/sports/basketball/thunder-down-grizzlies-anew-pacers-beat-bucks/</t>
+          <t>https://bilyonaryo.com/2025/05/02/slow-and-easily-beaten-messis-miami-project-risks-global-embarrassment/sports/</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A73" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8990 posts lower profit in 2024</t>
+          <t>Australian mushroom meal victim ‘hunched’ in pain, court hears</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/property/8990-posts-lower-profit-in-2024/</t>
+          <t>https://bilyonaryo.com/2025/05/02/australian-mushroom-meal-victim-hunched-in-pain-court-hears/food/</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A74" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>China asks Korea not to supply US with products using rare earths</t>
+          <t>Spain bans registration of overseas surrogate births</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/shipping-transportation/china-asks-korea-not-to-supply-us-with-products-using-rare-earths/</t>
+          <t>https://bilyonaryo.com/2025/05/02/spain-bans-registration-of-overseas-surrogate-births/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A75" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>ESG: Shaping the future of business and society</t>
+          <t>Rolls-Royce confident on profit targets despite tariffs</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/special-features/esg-shaping-the-future-of-business-and-society/</t>
+          <t>https://bilyonaryo.com/2025/05/02/rolls-royce-confident-on-profit-targets-despite-tariffs/trade/</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A76" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Vroom-vroom time: Two-wheel wonders roaring back</t>
+          <t>Billionaire Elon Musk admits DOGE cost-cutting drive falls short</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/motoring/vroom-vroom-time-two-wheel-wonders-roaring-back/</t>
+          <t>https://bilyonaryo.com/2025/05/02/billionaire-elon-musk-admits-doge-cost-cutting-drive-falls-short/money/</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A77" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Asthma Maintenance for Kids: Top Tips for Family Members</t>
+          <t>Microsoft raises Xbox prices globally, following Sony</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/lifestyle/asthma-maintenance-for-kids-top-tips-for-family-members/</t>
+          <t>https://bilyonaryo.com/2025/05/02/microsoft-raises-xbox-prices-globally-following-sony/technology/</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A78" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>New fashion brands find a home at SM’s Cebu malls</t>
+          <t>IKEA opens new London city center store</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/marketing-board/new-fashion-brands-find-a-home-at-sms-cebu-malls/</t>
+          <t>https://bilyonaryo.com/2025/05/02/ikea-opens-new-london-city-center-store/property/</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A79" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>NOTICE OF POSTPONEMENT OF ANNUAL STOCKHOLDERS’ MEETING</t>
+          <t>Rio Tinto has not fulfilled core pledge five years on from Juukan, Aboriginal group says</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/notices/notice-of-postponement-of-annual-stockholders-meeting/</t>
+          <t>https://bilyonaryo.com/2025/05/02/rio-tinto-has-not-fulfilled-core-pledge-five-years-on-from-juukan-aboriginal-group-says/mining/</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A80" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Haus Talk 2024 net income rises 51% to P365M</t>
+          <t>Virtual band PLAVE mixes K-pop and technology to charm fans</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/property/haus-talk-2024-net-income-rises-51-to-p365m/</t>
+          <t>https://bilyonaryo.com/2025/05/02/virtual-band-plave-mixes-k-pop-and-technology-to-charm-fans/entertainment/</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A81" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Oil prices extend climb</t>
+          <t>The Spanish state should take over grid operator, says deputy prime minister</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/business/shipping-transportation/oil-prices-extend-climb/</t>
+          <t>https://bilyonaryo.com/2025/05/02/the-spanish-state-should-take-over-grid-operator-says-deputy-prime-minister/power/</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A82" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>ESG: Shaping the future of business and society</t>
+          <t>Berkshire outguns market as Buffett reaches 60 years in charge</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/weekly-features/special-features/esg-shaping-the-future-of-business-and-society/</t>
+          <t>https://bilyonaryo.com/2025/05/02/berkshire-outguns-market-as-buffett-reaches-60-years-in-charge/money/</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A83" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Asthma Maintenance for Kids: Top Tips for Family Members</t>
+          <t>Will Italy get the papacy back after half a century of foreigners?</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/lifestyle/asthma-maintenance-for-kids-top-tips-for-family-members/</t>
+          <t>https://bilyonaryo.com/2025/05/02/will-italy-get-the-papacy-back-after-half-a-century-of-foreigners/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>April 24, 2025</t>
-        </is>
+      <c r="A84" s="3" t="n">
+        <v>45780</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Editorial Cartoon</t>
+          <t>KKR looks to deploy $116 billion cash in choppy market after profit boost</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://malaya.com.ph/opinion-of-the-day/editorial-cartoon/editorial-cartoon-143/</t>
+          <t>https://bilyonaryo.com/2025/05/02/kkr-looks-to-deploy-116-billion-cash-in-choppy-market-after-profit-boost/money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Tesla chair denies plans to look for new CEO to replace Musk</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/tesla-chair-denies-plans-to-look-for-new-ceo-to-replace-musk/mobility/</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Trump’s stablecoin chosen for $2 billion Abu Dhabi investment in Binance, co-founder says</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/trumps-stablecoin-chosen-for-2-billion-abu-dhabi-investment-in-binance-co-founder-says/money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Shell shock: Elche ban sunflower seed snacks in stadium clean-up act</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/shell-shock-elche-ban-sunflower-seed-snacks-in-stadium-clean-up-act/sports/</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CVS raises profit forecast, to exit Obamacare market as turnaround gains steam</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/cvs-raises-profit-forecast-to-exit-obamacare-market-as-turnaround-gains-steam/health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>‘Buena Vista Social Club,’ ‘Maybe Happy Ending’ and ‘Death Becomes Her’ lead 2025 Tony nominations</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/buena-vista-social-club-maybe-happy-ending-and-death-becomes-her-lead-2025-tony-nominations/lifestyle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Kuwait cracks down on cryptocurrency mining amid power crisis</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/kuwait-cracks-down-on-cryptocurrency-mining-amid-power-crisis/money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Bond market thinks Fed should cut rates, Treasury’s Bessent says</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/bond-market-thinks-fed-should-cut-rates-treasurys-bessent-says/money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>GM cuts 2025 profit forecast, expects up to $5 billion tariff impact</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/gm-cuts-2025-profit-forecast-expects-up-to-5-billion-tariff-impact/mobility/</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>WHO to back use of weight-loss drugs for adults globally, raises cost issue</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/who-to-back-use-of-weight-loss-drugs-for-adults-globally-raises-cost-issue/health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>No credit? No problem: Maya’s AI-powered Black Card has you covered</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/no-credit-no-problem-mayas-ai-powered-black-card-has-you-covered/money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>MVP’s Meralco eyes entry into Batangas amid resident discontent — can it  finally end frequent outages?</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/mvps-meralco-eyes-entry-into-batangas-amid-resident-discontent-can-it-finally-end-frequent-outages/power/</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Diversion lang: PNP drop Anson Que’s son from list of suspects for kidnap-slay case</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/diversion-lang-pnp-drop-anson-ques-son-from-list-of-suspects-for-kidnap-slay-case/business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Philippine police offer P5 million reward for suspect in businessman’s killing</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/philippine-police-offer-p5-million-reward-for-suspect-in-businessmans-killing/business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DOTr’s Vince Dizon to Cathay Pacific: Explain how a passport got shredded like junk mail</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/dotrs-vince-dizon-to-cathay-pacific-explain-how-a-passport-got-shredded-like-junk-mail/travel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Philippines’ Vice President Duterte says Marcos-ordered PrimeWater probe is political</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/philippines-vice-president-duterte-says-marcos-ordered-primewater-probe-is-political/business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Lopez-led First Gen seals geothermal supply deal Cebu’s Chioson Group</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://bilyonaryo.com/2025/05/02/lopez-led-first-gen-seals-geothermal-supply-deal-cebus-chioson-group/power/</t>
         </is>
       </c>
     </row>
@@ -1946,6 +2024,22 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C82" r:id="rId81"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C83" r:id="rId82"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C84" r:id="rId83"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C85" r:id="rId84"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C86" r:id="rId85"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C87" r:id="rId86"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C88" r:id="rId87"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C89" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C90" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C91" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C92" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C93" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C94" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C95" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C96" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C97" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C98" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C99" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C100" r:id="rId99"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>